<commit_message>
finish nested benders experiment for 5 years
</commit_message>
<xml_diff>
--- a/small_test.xlsx
+++ b/small_test.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="37880" windowHeight="19380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19400" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test case" sheetId="1" r:id="rId1"/>
-    <sheet name="5years" sheetId="2" r:id="rId2"/>
+    <sheet name="5years gtep" sheetId="2" r:id="rId2"/>
+    <sheet name="5 years gep" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="84">
   <si>
     <t>{1: 181.810526013149, 2: 184.34769990276584, 3: 191.85019162638417, 4: 194.4695006297496, 5: 195.9107171894354, 6: 197.47855713927356, 7: 198.19404218211034, 8: 198.60493506211662, 9: 198.84753703487908}</t>
   </si>
@@ -179,6 +180,108 @@
   </si>
   <si>
     <t>LB: 85.4111</t>
+  </si>
+  <si>
+    <t>theta values</t>
+  </si>
+  <si>
+    <t>0.1 - 0.2</t>
+  </si>
+  <si>
+    <t>Time: 252 secs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UB: 87.0907  </t>
+  </si>
+  <si>
+    <t>LB: 86.5042</t>
+  </si>
+  <si>
+    <t>[8.581202550356048</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17.7517514797149]</t>
+  </si>
+  <si>
+    <t>[2.2216852157074682</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.7903493607715788]</t>
+  </si>
+  <si>
+    <t>[0.008933514358984132</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.04470861629619455]</t>
+  </si>
+  <si>
+    <t>[0.3933761981860087</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.14122426181963946]</t>
+  </si>
+  <si>
+    <t>[0.05451008066027791</t>
+  </si>
+  <si>
+    <t>[0.030525828066020638</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.1003510612734374]</t>
+  </si>
+  <si>
+    <t>[3483.4180645445267</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3483.4180645445267]</t>
+  </si>
+  <si>
+    <t>[75787.901</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 76797.901]</t>
+  </si>
+  <si>
+    <t>[79271.31906454453</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 80281.31906454453]</t>
+  </si>
+  <si>
+    <t>mostly 500kv tielines are installed</t>
+  </si>
+  <si>
+    <t>solve with nested Benders</t>
+  </si>
+  <si>
+    <t>{1: 65.17623593479956, 2: 65.3288786465648, 3: 68.95738937437396, 4: 65.93661149792841, 5: 68.20880719512733, 6: 65.96511814562481, 7: 66.16349861974903, 8: 66.41984385295665, 9: 66.53960819055625, 10: 66.10504872355017, 11: 66.17189303802222, 12: 66.57432103323951, 13: 67.24897669753358, 14: 66.76216205591733, 15: 66.03212077272534, 16: 66.29213536431064, 17: 65.72804980503211, 18: 68.10367972041138, 19: 67.79153526288226, 20: 66.68454067481242, 21: 68.72877167212017, 22: 68.63595858553, 23: 66.13727358624301, 24: 67.27065308470976, 25: 68.76702695352998, 26: 67.47226698474773, 27: 71.20037606659108}</t>
+  </si>
+  <si>
+    <t>gap:  20.86706222252392</t>
+  </si>
+  <si>
+    <t>CPU Time (s) 42125.97545313835</t>
+  </si>
+  <si>
+    <t>LB</t>
+  </si>
+  <si>
+    <t>UB</t>
+  </si>
+  <si>
+    <t>{1: 89.9756511843506, 2: 89.9756511843506, 3: 89.9756511843506, 4: 89.9756511843506, 5: 89.9756511843506, 6: 89.9756511843506, 7: 89.9756511843506, 8: 89.9756511843506, 9: 89.9756511843506, 10: 89.9756511843506, 11: 89.9756511843506, 12: 89.9756511843506, 13: 89.9756511843506, 14: 89.9756511843506, 15: 89.9756511843506, 16: 89.9756511843506, 17: 89.9756511843506, 18: 89.9756511843506, 19: 89.9756511843506, 20: 89.9756511843506, 21: 89.9756511843506, 22: 89.9756511843506, 23: 89.9756511843506, 24: 89.9756511843506, 25: 89.9756511843506, 26: 89.9756511843506, 27: 89.9756511843506}</t>
+  </si>
+  <si>
+    <t>Upper Bound 86.84551447227336</t>
+  </si>
+  <si>
+    <t>Lower Bound 86.25202879972517</t>
+  </si>
+  <si>
+    <t>Optimality gap (%) 0.6833809162794198</t>
+  </si>
+  <si>
+    <t>CPU Time (s) 3892.179146051407</t>
   </si>
 </sst>
 </file>
@@ -227,8 +330,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -241,11 +364,31 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -523,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -598,14 +741,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.83203125" customWidth="1"/>
+    <col min="10" max="10" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -646,6 +790,9 @@
       <c r="E3" t="s">
         <v>27</v>
       </c>
+      <c r="K3" s="2">
+        <v>83.793783513999998</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -673,11 +820,20 @@
       <c r="E6" t="s">
         <v>29</v>
       </c>
+      <c r="I6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>10.1571680388065</v>
       </c>
+      <c r="I7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -705,11 +861,23 @@
       <c r="A10">
         <v>0.289386499423054</v>
       </c>
+      <c r="I10" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
+      <c r="H11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11">
+        <v>71.2</v>
+      </c>
+      <c r="J11" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -727,16 +895,31 @@
       <c r="E12" t="s">
         <v>33</v>
       </c>
+      <c r="H12" t="s">
+        <v>78</v>
+      </c>
+      <c r="I12">
+        <v>89.97</v>
+      </c>
+      <c r="J12" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4.5628694585030001</v>
       </c>
+      <c r="I13" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
+      <c r="I14" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -978,5 +1161,377 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M39"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5">
+        <v>15.126321236286699</v>
+      </c>
+      <c r="C5">
+        <v>16.112845377106499</v>
+      </c>
+      <c r="D5">
+        <v>16.806105476646401</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>74.378226120110597</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8">
+        <v>2.1128402076147301</v>
+      </c>
+      <c r="C8">
+        <v>1.9988994890038601</v>
+      </c>
+      <c r="D8">
+        <v>1.89240236025252</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>10.016176633350099</v>
+      </c>
+      <c r="K9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11">
+        <v>4.0584896073915099E-2</v>
+      </c>
+      <c r="C11">
+        <v>4.9115013295807398E-2</v>
+      </c>
+      <c r="D11">
+        <v>4.7554158316280098E-2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0.19089619834118099</v>
+      </c>
+      <c r="K12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14">
+        <v>1.0648145441655199</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0.20356306061628199</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1.2683776047818101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17">
+        <v>4.3276503274884102E-2</v>
+      </c>
+      <c r="C17">
+        <v>1.3129056926889499E-2</v>
+      </c>
+      <c r="D17">
+        <v>1.20821269488323E-2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>0.60308814715625403</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>5.4510080660277897E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>7.1407274669493996E-3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>7.1407274669493996E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26">
+        <v>0.129725234657626</v>
+      </c>
+      <c r="C26">
+        <v>0.22907041047450999</v>
+      </c>
+      <c r="D26">
+        <v>8.2658613170886103E-2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>0.57233114764248105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32">
+        <v>3483.4180645445199</v>
+      </c>
+      <c r="C32">
+        <v>3483.4180645445199</v>
+      </c>
+      <c r="D32">
+        <v>3483.4180645445199</v>
+      </c>
+      <c r="E32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>17417.090322722601</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35">
+        <v>76587.900999999998</v>
+      </c>
+      <c r="C35">
+        <v>76587.900999999998</v>
+      </c>
+      <c r="D35">
+        <v>76797.900999999998</v>
+      </c>
+      <c r="E35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>382559.505</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38">
+        <v>80071.319064544499</v>
+      </c>
+      <c r="C38">
+        <v>80071.319064544499</v>
+      </c>
+      <c r="D38">
+        <v>80281.319064544499</v>
+      </c>
+      <c r="E38" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>399976.59532272199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
try benders using python api
</commit_message>
<xml_diff>
--- a/small_test.xlsx
+++ b/small_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19400" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="38440" yWindow="460" windowWidth="38400" windowHeight="19400" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test case" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="85">
   <si>
     <t>{1: 181.810526013149, 2: 184.34769990276584, 3: 191.85019162638417, 4: 194.4695006297496, 5: 195.9107171894354, 6: 197.47855713927356, 7: 198.19404218211034, 8: 198.60493506211662, 9: 198.84753703487908}</t>
   </si>
@@ -282,6 +282,9 @@
   </si>
   <si>
     <t>CPU Time (s) 3892.179146051407</t>
+  </si>
+  <si>
+    <t>LP relaxation</t>
   </si>
 </sst>
 </file>
@@ -739,10 +742,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -752,7 +755,7 @@
     <col min="10" max="10" width="29.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -763,7 +766,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -774,7 +777,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -793,18 +796,22 @@
       <c r="K3" s="2">
         <v>83.793783513999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" s="2">
+        <f>(86.23-K3)/K3</f>
+        <v>2.9073952551539474E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>64.199285979304506</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -827,7 +834,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>10.1571680388065</v>
       </c>
@@ -835,12 +842,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -857,7 +864,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.289386499423054</v>
       </c>
@@ -865,7 +872,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -879,7 +886,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -905,7 +912,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4.5628694585030001</v>
       </c>
@@ -913,7 +920,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -921,7 +928,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -938,7 +945,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.39978867830481202</v>
       </c>
@@ -1169,8 +1176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1191,9 +1198,17 @@
         <v>54</v>
       </c>
     </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
+      </c>
+      <c r="L4">
+        <v>86.43</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
get benders working using cplex strategy 2
</commit_message>
<xml_diff>
--- a/small_test.xlsx
+++ b/small_test.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38440" yWindow="460" windowWidth="38400" windowHeight="19400" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="33600" windowHeight="19400" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test case" sheetId="1" r:id="rId1"/>
     <sheet name="5years gtep" sheetId="2" r:id="rId2"/>
-    <sheet name="5 years gep" sheetId="3" r:id="rId3"/>
+    <sheet name="5years gtep benders" sheetId="4" r:id="rId3"/>
+    <sheet name="5 years gep" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="200">
   <si>
     <t>{1: 181.810526013149, 2: 184.34769990276584, 3: 191.85019162638417, 4: 194.4695006297496, 5: 195.9107171894354, 6: 197.47855713927356, 7: 198.19404218211034, 8: 198.60493506211662, 9: 198.84753703487908}</t>
   </si>
@@ -285,6 +286,351 @@
   </si>
   <si>
     <t>LP relaxation</t>
+  </si>
+  <si>
+    <t>put all the investment decisions in the master problem</t>
+  </si>
+  <si>
+    <t>CPXPARAM_Read_DataCheck                          1</t>
+  </si>
+  <si>
+    <t>CPXPARAM_Benders_Strategy                        2</t>
+  </si>
+  <si>
+    <t>CPXPARAM_MIP_Tolerances_MIPGap                   0.01</t>
+  </si>
+  <si>
+    <t>Tried aggregator 2 times.</t>
+  </si>
+  <si>
+    <t>MIP Presolve eliminated 55461 rows and 30277 columns.</t>
+  </si>
+  <si>
+    <t>MIP Presolve modified 74919 coefficients.</t>
+  </si>
+  <si>
+    <t>Aggregator did 1280 substitutions.</t>
+  </si>
+  <si>
+    <t>Reduced MIP has 321118 rows, 181733 columns, and 1069173 nonzeros.</t>
+  </si>
+  <si>
+    <t>Reduced MIP has 595 binaries, 419 generals, 0 SOSs, and 0 indicators.</t>
+  </si>
+  <si>
+    <t>Presolve time = 1.46 sec. (557.30 ticks)</t>
+  </si>
+  <si>
+    <t>Tried aggregator 1 time.</t>
+  </si>
+  <si>
+    <t>Presolve time = 0.50 sec. (307.03 ticks)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Nodes                                         Cuts/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Node  Left     Objective  IInf  Best Integer    Best Bound    ItCnt     Gap</t>
+  </si>
+  <si>
+    <t>MIP Presolve eliminated 113 rows and 0 columns.</t>
+  </si>
+  <si>
+    <t>Aggregator did 16 substitutions.</t>
+  </si>
+  <si>
+    <t>Reduced MIP has 577 rows, 1275 columns, and 3803 nonzeros.</t>
+  </si>
+  <si>
+    <t>Reduced MIP has 585 binaries, 414 generals, 0 SOSs, and 0 indicators.</t>
+  </si>
+  <si>
+    <t>Presolve time = 0.00 sec. (2.24 ticks)</t>
+  </si>
+  <si>
+    <t>Probing time = 0.00 sec. (0.19 ticks)</t>
+  </si>
+  <si>
+    <t>Presolve time = 0.00 sec. (1.03 ticks)</t>
+  </si>
+  <si>
+    <t>Clique table members: 153.</t>
+  </si>
+  <si>
+    <t>MIP emphasis: balance optimality and feasibility.</t>
+  </si>
+  <si>
+    <t>MIP search method: dynamic search.</t>
+  </si>
+  <si>
+    <t>Parallel mode: deterministic, using up to 24 threads.</t>
+  </si>
+  <si>
+    <t>Root relaxation solution time = 0.01 sec. (9.00 ticks)</t>
+  </si>
+  <si>
+    <t>*     0+    0                          164.4229       84.6334            48.53%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.5364    35      164.4229       84.6334     2493   48.53%</t>
+  </si>
+  <si>
+    <t>*     0+    0                           86.9963       84.6334             2.72%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.6274    41       86.9963      Cuts: 17     2505    2.72%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.6682    28       86.9963       Cuts: 7     2514    2.68%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.7275    44       86.9963       Cuts: 4     2527    2.61%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.7825    41       86.9963       Cuts: 5     2542    2.54%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.7909    42       86.9963       Cuts: 7     2549    2.54%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.7998    47       86.9963       Cuts: 5     2555    2.52%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.8228    63       86.9963      Cuts: 10     2567    2.50%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.8272    70       86.9963       Cuts: 8     2574    2.49%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.8377    52       86.9963       Cuts: 5     2583    2.48%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.8501    64       86.9963       Cuts: 5     2595    2.47%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.8534    65       86.9963    MIRcuts: 2     2600    2.46%</t>
+  </si>
+  <si>
+    <t>Heuristic still looking.</t>
+  </si>
+  <si>
+    <t>Repeating presolve.</t>
+  </si>
+  <si>
+    <t>MIP Presolve eliminated 95 rows and 195 columns.</t>
+  </si>
+  <si>
+    <t>Reduced MIP has 482 rows, 1080 columns, and 3130 nonzeros.</t>
+  </si>
+  <si>
+    <t>Reduced MIP has 585 binaries, 219 generals, 0 SOSs, and 0 indicators.</t>
+  </si>
+  <si>
+    <t>Presolve time = 0.00 sec. (1.02 ticks)</t>
+  </si>
+  <si>
+    <t>Presolve time = 0.00 sec. (0.92 ticks)</t>
+  </si>
+  <si>
+    <t>Represolve time = 0.30 sec. (52.08 ticks)</t>
+  </si>
+  <si>
+    <t>Root relaxation solution time = 0.02 sec. (11.32 ticks)</t>
+  </si>
+  <si>
+    <t>*     0+    0                           86.9963       84.8534             2.46%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.8548    61       86.9963       84.8548     5016    2.46%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.8621    66       86.9963    MIRcuts: 5     5021    2.45%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.8644    65       86.9963    MIRcuts: 3     5025    2.45%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.8720    68       86.9963    MIRcuts: 5     5033    2.44%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.8792    68       86.9963    MIRcuts: 3     5038    2.43%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     2       84.8792    68       86.9963       84.8792     5038    2.43%</t>
+  </si>
+  <si>
+    <t>Elapsed time = 1051.74 sec. (720985.05 ticks, tree = 0.02 MB, solutions = 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     10     6       85.3863    31       86.9963       84.9058     5114    2.40%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     40     7       85.9319    41       86.9963       84.9058     5115    2.40%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     50    17       85.7654    43       86.9963       84.9058     5188    2.40%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     60    25       86.2581    35       86.9963       84.9058     5260    2.40%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     88    23       86.0420    39       86.9963       84.9058     5230    2.40%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    116     9       86.3650    50       86.9963       84.9058     5128    2.40%</t>
+  </si>
+  <si>
+    <t>*   117+   12                           86.9206       84.9058             2.32%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    117    14       85.5483    42       86.9206       84.9058     5175    2.32%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    127    37       86.2488    19       86.9206       84.9058     5314    2.32%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    154    12       86.4334    34       86.9206       84.9058     5155    2.32%</t>
+  </si>
+  <si>
+    <t>*   180+    1                           86.2425       84.9058             1.55%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    180     3       85.0615    59       86.2425       84.9058     5054    1.55%</t>
+  </si>
+  <si>
+    <t>Elapsed time = 1163.30 sec. (749608.56 ticks, tree = 0.02 MB, solutions = 3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    190    38       86.2608    20       86.2425       84.9095     5339    1.55%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    192    79       86.5992    13       86.2425       84.9095     5579    1.55%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    268    10       86.2752    43       86.2425       84.9095     5135    1.55%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    303    24       86.4922    28       86.2425       84.9839     5237    1.46%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    304    60       86.0380    36       86.2425       84.9839     5527    1.46%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    434    80       86.1822    10       86.2425       84.9839     6126    1.46%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    498   155       85.3077    70       86.2425       84.9850     7413    1.46%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    622    63       85.7543    29       86.2425       84.9850     5909    1.46%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    638    22       86.1642    32       86.2425       84.9850     5219    1.46%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    698    69       86.0840     0       86.2425       84.9850     6032    1.46%</t>
+  </si>
+  <si>
+    <t>Elapsed time = 1226.68 sec. (765274.53 ticks, tree = 0.04 MB, solutions = 4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    704   134       86.1581     8       86.2425       84.9850     6874    1.46%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    862   143       86.0460    19       86.2425       84.9850     7175    1.46%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    951   141       85.7609    17       86.2425       84.9850     7098    1.46%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1012   169       85.7433    30       86.2425       85.0580     7937    1.37%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1019    59       85.8884    28       86.2425       85.0580     5584    1.37%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1095   307       85.3725    32       86.2425       85.0580     9628    1.37%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1118    13       85.8771    38       86.2425       85.0580     5169    1.37%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1120   171       86.1309    14       86.2425       85.0580     7823    1.37%</t>
+  </si>
+  <si>
+    <t>*  1266+  320                           85.9576       85.0580             1.05%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1267   488        cutoff             85.9576       85.0580    12166    1.05%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1273   472       86.0835     5       85.9576       85.0580    11961    1.05%</t>
+  </si>
+  <si>
+    <t>Elapsed time = 1271.20 sec. (779316.59 ticks, tree = 0.42 MB, solutions = 6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1288   474       86.2229    27       85.9576       85.0580    11964    1.05%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1289   450       85.8875    13       85.9576       85.0580    11921    1.05%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1293   512        cutoff             85.9576       85.0580    12304    1.05%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1294   544        cutoff             85.9576       85.0580    12576    1.05%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   1295   551        cutoff             85.9576       85.0580    12591    1.05%</t>
+  </si>
+  <si>
+    <t>Benders cuts applied:  1013</t>
+  </si>
+  <si>
+    <t>Mixed integer rounding cuts applied:  27</t>
+  </si>
+  <si>
+    <t>Gomory fractional cuts applied:  3</t>
+  </si>
+  <si>
+    <t>Root node processing (before b&amp;c):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Real time             = 1046.52 sec. (720956.77 ticks)</t>
+  </si>
+  <si>
+    <t>Parallel b&amp;c, 24 threads:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Real time             =  239.00 sec. (68244.73 ticks)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Sync time (average)   =   27.04 sec.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wait time (average)   =    0.00 sec.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          ------------</t>
+  </si>
+  <si>
+    <t>Total (root+branch&amp;cut) = 1285.52 sec. (789201.51 ticks)</t>
+  </si>
+  <si>
+    <t>Lower bound</t>
+  </si>
+  <si>
+    <t>Upper bound</t>
+  </si>
+  <si>
+    <t>Cplex Benders time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upper bound time </t>
+  </si>
+  <si>
+    <t>gap</t>
   </si>
 </sst>
 </file>
@@ -745,7 +1091,7 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1174,9 +1520,715 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K136"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H1" t="s">
+        <v>196</v>
+      </c>
+      <c r="I1" t="s">
+        <v>197</v>
+      </c>
+      <c r="J1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2">
+        <v>85.207300000000004</v>
+      </c>
+      <c r="H2">
+        <v>86.247</v>
+      </c>
+      <c r="I2">
+        <v>1285</v>
+      </c>
+      <c r="J2">
+        <v>20</v>
+      </c>
+      <c r="K2">
+        <f>(H2-G2)/H2</f>
+        <v>1.2054912054912012E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>194</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
benders cplex work for gtep
</commit_message>
<xml_diff>
--- a/small_test.xlsx
+++ b/small_test.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="175">
   <si>
     <t>{1: 181.810526013149, 2: 184.34769990276584, 3: 191.85019162638417, 4: 194.4695006297496, 5: 195.9107171894354, 6: 197.47855713927356, 7: 198.19404218211034, 8: 198.60493506211662, 9: 198.84753703487908}</t>
   </si>
@@ -303,60 +303,18 @@
     <t>Tried aggregator 2 times.</t>
   </si>
   <si>
-    <t>MIP Presolve eliminated 55461 rows and 30277 columns.</t>
-  </si>
-  <si>
     <t>MIP Presolve modified 74919 coefficients.</t>
   </si>
   <si>
-    <t>Aggregator did 1280 substitutions.</t>
-  </si>
-  <si>
-    <t>Reduced MIP has 321118 rows, 181733 columns, and 1069173 nonzeros.</t>
-  </si>
-  <si>
-    <t>Reduced MIP has 595 binaries, 419 generals, 0 SOSs, and 0 indicators.</t>
-  </si>
-  <si>
-    <t>Presolve time = 1.46 sec. (557.30 ticks)</t>
-  </si>
-  <si>
     <t>Tried aggregator 1 time.</t>
   </si>
   <si>
-    <t>Presolve time = 0.50 sec. (307.03 ticks)</t>
-  </si>
-  <si>
     <t xml:space="preserve">        Nodes                                         Cuts/</t>
   </si>
   <si>
     <t xml:space="preserve">   Node  Left     Objective  IInf  Best Integer    Best Bound    ItCnt     Gap</t>
   </si>
   <si>
-    <t>MIP Presolve eliminated 113 rows and 0 columns.</t>
-  </si>
-  <si>
-    <t>Aggregator did 16 substitutions.</t>
-  </si>
-  <si>
-    <t>Reduced MIP has 577 rows, 1275 columns, and 3803 nonzeros.</t>
-  </si>
-  <si>
-    <t>Reduced MIP has 585 binaries, 414 generals, 0 SOSs, and 0 indicators.</t>
-  </si>
-  <si>
-    <t>Presolve time = 0.00 sec. (2.24 ticks)</t>
-  </si>
-  <si>
-    <t>Probing time = 0.00 sec. (0.19 ticks)</t>
-  </si>
-  <si>
-    <t>Presolve time = 0.00 sec. (1.03 ticks)</t>
-  </si>
-  <si>
-    <t>Clique table members: 153.</t>
-  </si>
-  <si>
     <t>MIP emphasis: balance optimality and feasibility.</t>
   </si>
   <si>
@@ -366,258 +324,27 @@
     <t>Parallel mode: deterministic, using up to 24 threads.</t>
   </si>
   <si>
-    <t>Root relaxation solution time = 0.01 sec. (9.00 ticks)</t>
-  </si>
-  <si>
-    <t>*     0+    0                          164.4229       84.6334            48.53%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      0     0       84.5364    35      164.4229       84.6334     2493   48.53%</t>
-  </si>
-  <si>
-    <t>*     0+    0                           86.9963       84.6334             2.72%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      0     0       84.6274    41       86.9963      Cuts: 17     2505    2.72%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      0     0       84.6682    28       86.9963       Cuts: 7     2514    2.68%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      0     0       84.7275    44       86.9963       Cuts: 4     2527    2.61%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      0     0       84.7825    41       86.9963       Cuts: 5     2542    2.54%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      0     0       84.7909    42       86.9963       Cuts: 7     2549    2.54%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      0     0       84.7998    47       86.9963       Cuts: 5     2555    2.52%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      0     0       84.8228    63       86.9963      Cuts: 10     2567    2.50%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      0     0       84.8272    70       86.9963       Cuts: 8     2574    2.49%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      0     0       84.8377    52       86.9963       Cuts: 5     2583    2.48%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      0     0       84.8501    64       86.9963       Cuts: 5     2595    2.47%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      0     0       84.8534    65       86.9963    MIRcuts: 2     2600    2.46%</t>
-  </si>
-  <si>
     <t>Heuristic still looking.</t>
   </si>
   <si>
     <t>Repeating presolve.</t>
   </si>
   <si>
-    <t>MIP Presolve eliminated 95 rows and 195 columns.</t>
-  </si>
-  <si>
-    <t>Reduced MIP has 482 rows, 1080 columns, and 3130 nonzeros.</t>
-  </si>
-  <si>
-    <t>Reduced MIP has 585 binaries, 219 generals, 0 SOSs, and 0 indicators.</t>
-  </si>
-  <si>
-    <t>Presolve time = 0.00 sec. (1.02 ticks)</t>
-  </si>
-  <si>
-    <t>Presolve time = 0.00 sec. (0.92 ticks)</t>
-  </si>
-  <si>
-    <t>Represolve time = 0.30 sec. (52.08 ticks)</t>
-  </si>
-  <si>
-    <t>Root relaxation solution time = 0.02 sec. (11.32 ticks)</t>
-  </si>
-  <si>
-    <t>*     0+    0                           86.9963       84.8534             2.46%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      0     0       84.8548    61       86.9963       84.8548     5016    2.46%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      0     0       84.8621    66       86.9963    MIRcuts: 5     5021    2.45%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      0     0       84.8644    65       86.9963    MIRcuts: 3     5025    2.45%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      0     0       84.8720    68       86.9963    MIRcuts: 5     5033    2.44%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      0     0       84.8792    68       86.9963    MIRcuts: 3     5038    2.43%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      0     2       84.8792    68       86.9963       84.8792     5038    2.43%</t>
-  </si>
-  <si>
-    <t>Elapsed time = 1051.74 sec. (720985.05 ticks, tree = 0.02 MB, solutions = 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     10     6       85.3863    31       86.9963       84.9058     5114    2.40%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     40     7       85.9319    41       86.9963       84.9058     5115    2.40%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     50    17       85.7654    43       86.9963       84.9058     5188    2.40%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     60    25       86.2581    35       86.9963       84.9058     5260    2.40%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     88    23       86.0420    39       86.9963       84.9058     5230    2.40%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    116     9       86.3650    50       86.9963       84.9058     5128    2.40%</t>
-  </si>
-  <si>
-    <t>*   117+   12                           86.9206       84.9058             2.32%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    117    14       85.5483    42       86.9206       84.9058     5175    2.32%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    127    37       86.2488    19       86.9206       84.9058     5314    2.32%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    154    12       86.4334    34       86.9206       84.9058     5155    2.32%</t>
-  </si>
-  <si>
-    <t>*   180+    1                           86.2425       84.9058             1.55%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    180     3       85.0615    59       86.2425       84.9058     5054    1.55%</t>
-  </si>
-  <si>
-    <t>Elapsed time = 1163.30 sec. (749608.56 ticks, tree = 0.02 MB, solutions = 3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    190    38       86.2608    20       86.2425       84.9095     5339    1.55%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    192    79       86.5992    13       86.2425       84.9095     5579    1.55%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    268    10       86.2752    43       86.2425       84.9095     5135    1.55%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    303    24       86.4922    28       86.2425       84.9839     5237    1.46%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    304    60       86.0380    36       86.2425       84.9839     5527    1.46%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    434    80       86.1822    10       86.2425       84.9839     6126    1.46%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    498   155       85.3077    70       86.2425       84.9850     7413    1.46%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    622    63       85.7543    29       86.2425       84.9850     5909    1.46%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    638    22       86.1642    32       86.2425       84.9850     5219    1.46%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    698    69       86.0840     0       86.2425       84.9850     6032    1.46%</t>
-  </si>
-  <si>
-    <t>Elapsed time = 1226.68 sec. (765274.53 ticks, tree = 0.04 MB, solutions = 4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    704   134       86.1581     8       86.2425       84.9850     6874    1.46%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    862   143       86.0460    19       86.2425       84.9850     7175    1.46%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    951   141       85.7609    17       86.2425       84.9850     7098    1.46%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1012   169       85.7433    30       86.2425       85.0580     7937    1.37%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1019    59       85.8884    28       86.2425       85.0580     5584    1.37%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1095   307       85.3725    32       86.2425       85.0580     9628    1.37%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1118    13       85.8771    38       86.2425       85.0580     5169    1.37%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1120   171       86.1309    14       86.2425       85.0580     7823    1.37%</t>
-  </si>
-  <si>
-    <t>*  1266+  320                           85.9576       85.0580             1.05%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1267   488        cutoff             85.9576       85.0580    12166    1.05%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1273   472       86.0835     5       85.9576       85.0580    11961    1.05%</t>
-  </si>
-  <si>
-    <t>Elapsed time = 1271.20 sec. (779316.59 ticks, tree = 0.42 MB, solutions = 6)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1288   474       86.2229    27       85.9576       85.0580    11964    1.05%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1289   450       85.8875    13       85.9576       85.0580    11921    1.05%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1293   512        cutoff             85.9576       85.0580    12304    1.05%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1294   544        cutoff             85.9576       85.0580    12576    1.05%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1295   551        cutoff             85.9576       85.0580    12591    1.05%</t>
-  </si>
-  <si>
-    <t>Benders cuts applied:  1013</t>
-  </si>
-  <si>
-    <t>Mixed integer rounding cuts applied:  27</t>
-  </si>
-  <si>
     <t>Gomory fractional cuts applied:  3</t>
   </si>
   <si>
     <t>Root node processing (before b&amp;c):</t>
   </si>
   <si>
-    <t xml:space="preserve">  Real time             = 1046.52 sec. (720956.77 ticks)</t>
-  </si>
-  <si>
     <t>Parallel b&amp;c, 24 threads:</t>
   </si>
   <si>
-    <t xml:space="preserve">  Real time             =  239.00 sec. (68244.73 ticks)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Sync time (average)   =   27.04 sec.</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Wait time (average)   =    0.00 sec.</t>
   </si>
   <si>
     <t xml:space="preserve">                          ------------</t>
   </si>
   <si>
-    <t>Total (root+branch&amp;cut) = 1285.52 sec. (789201.51 ticks)</t>
-  </si>
-  <si>
     <t>Lower bound</t>
   </si>
   <si>
@@ -631,6 +358,204 @@
   </si>
   <si>
     <t>gap</t>
+  </si>
+  <si>
+    <t>MIP Presolve eliminated 55461 rows and 30397 columns.</t>
+  </si>
+  <si>
+    <t>Aggregator did 1827 substitutions.</t>
+  </si>
+  <si>
+    <t>Reduced MIP has 320571 rows, 181066 columns, and 1067959 nonzeros.</t>
+  </si>
+  <si>
+    <t>Reduced MIP has 595 binaries, 279 generals, 0 SOSs, and 0 indicators.</t>
+  </si>
+  <si>
+    <t>Presolve time = 1.26 sec. (590.02 ticks)</t>
+  </si>
+  <si>
+    <t>Presolve time = 0.50 sec. (306.91 ticks)</t>
+  </si>
+  <si>
+    <t>Aggregator did 73 substitutions.</t>
+  </si>
+  <si>
+    <t>Reduced MIP has 497 rows, 1082 columns, and 3767 nonzeros.</t>
+  </si>
+  <si>
+    <t>Reduced MIP has 553 binaries, 279 generals, 0 SOSs, and 0 indicators.</t>
+  </si>
+  <si>
+    <t>Presolve time = 0.00 sec. (1.84 ticks)</t>
+  </si>
+  <si>
+    <t>Probing time = 0.00 sec. (0.53 ticks)</t>
+  </si>
+  <si>
+    <t>Presolve time = 0.00 sec. (0.99 ticks)</t>
+  </si>
+  <si>
+    <t>Clique table members: 1470.</t>
+  </si>
+  <si>
+    <t>Root relaxation solution time = 0.02 sec. (7.68 ticks)</t>
+  </si>
+  <si>
+    <t>*     0+    0                          160.3901       84.7569            47.16%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.7660    31      160.3901       84.7660      743   47.15%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.9033    27      160.3901      Cuts: 16      754   47.06%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.9452    46      160.3901       Cuts: 6      761   47.04%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.9636    59      160.3901       Cuts: 6      771   47.03%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.9656    54      160.3901       Cuts: 5      776   47.03%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.9713    55      160.3901       Cuts: 5      788   47.02%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.9765    49      160.3901    MIRcuts: 3      794   47.02%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.9824    46      160.3901    MIRcuts: 1      798   47.02%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.9856    56      160.3901    Benders: 1      801   47.01%</t>
+  </si>
+  <si>
+    <t>*     0+    0                           87.0895       84.9856             2.42%</t>
+  </si>
+  <si>
+    <t>*     0+    0                           86.2017       84.9856             1.41%</t>
+  </si>
+  <si>
+    <t>MIP Presolve eliminated 95 rows and 135 columns.</t>
+  </si>
+  <si>
+    <t>Reduced MIP has 402 rows, 947 columns, and 3160 nonzeros.</t>
+  </si>
+  <si>
+    <t>Reduced MIP has 566 binaries, 131 generals, 0 SOSs, and 0 indicators.</t>
+  </si>
+  <si>
+    <t>Presolve time = 0.00 sec. (0.96 ticks)</t>
+  </si>
+  <si>
+    <t>Probing time = 0.00 sec. (0.54 ticks)</t>
+  </si>
+  <si>
+    <t>Presolve time = 0.00 sec. (0.89 ticks)</t>
+  </si>
+  <si>
+    <t>Represolve time = 0.07 sec. (28.61 ticks)</t>
+  </si>
+  <si>
+    <t>Root relaxation solution time = 0.01 sec. (6.18 ticks)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.9884    52       86.2017       84.9884     1504    1.41%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.9989    61       86.2017       Cuts: 5     1514    1.40%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       84.9998    63       86.2017    MIRcuts: 1     1516    1.39%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     0       85.0016    64       86.2017    MIRcuts: 1     1517    1.39%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      0     2       85.0016    64       86.2017       85.0016     1517    1.39%</t>
+  </si>
+  <si>
+    <t>Elapsed time = 588.79 sec. (399211.44 ticks, tree = 0.02 MB, solutions = 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     51    16       85.4144    27       86.2017       85.0143     1648    1.38%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     53    15       85.2773    32       86.2017       85.0143     1643    1.38%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     66    18       85.2327    33       86.2017       85.0143     1676    1.38%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     74    27       85.2947    14       86.2017       85.0143     1721    1.38%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     75     5       85.0158    38       86.2017       85.0143     1530    1.38%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     85    11       85.3566    20       86.2017       85.0514     1591    1.33%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     86    19       85.3008    31       86.2017       85.0514     1683    1.33%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     96    27       85.6648    24       86.2017       85.0514     1728    1.33%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     97    65       85.9238    12       86.2017       85.0514     2163    1.33%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    100    17       85.2948    36       86.2017       85.0514     1654    1.33%</t>
+  </si>
+  <si>
+    <t>Elapsed time = 648.62 sec. (416043.18 ticks, tree = 0.02 MB, solutions = 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    137    51       85.7478    30       86.2017       85.0514     2040    1.33%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    139    31       85.2773    11       86.2017       85.0514     1806    1.33%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    163    72       85.6340    11       86.2017       85.0514     2179    1.33%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    207     8       85.2564    24       86.2017       85.1800     1574    1.19%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    211    97        cutoff             86.2017       85.2505     2340    1.10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    213   104        cutoff             86.2017       85.2505     2428    1.10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    216   144       85.8891    11       86.2017       85.2505     2947    1.10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    222   154        cutoff             86.2017       85.2723     3019    1.08%</t>
+  </si>
+  <si>
+    <t>Benders cuts applied:  179</t>
+  </si>
+  <si>
+    <t>Mixed integer rounding cuts applied:  24</t>
+  </si>
+  <si>
+    <t>Lift and project cuts applied:  1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Real time             =  586.88 sec. (399190.70 ticks)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Real time             =   98.13 sec. (42324.87 ticks)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Sync time (average)   =   44.18 sec.</t>
+  </si>
+  <si>
+    <t>Total (root+branch&amp;cut) =  685.01 sec. (441515.57 ticks)</t>
   </si>
 </sst>
 </file>
@@ -1520,10 +1445,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K136"/>
+  <dimension ref="A1:K113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1538,19 +1463,19 @@
         <v>85</v>
       </c>
       <c r="G1" t="s">
-        <v>195</v>
+        <v>104</v>
       </c>
       <c r="H1" t="s">
-        <v>196</v>
+        <v>105</v>
       </c>
       <c r="I1" t="s">
-        <v>197</v>
+        <v>106</v>
       </c>
       <c r="J1" t="s">
-        <v>198</v>
+        <v>107</v>
       </c>
       <c r="K1" t="s">
-        <v>199</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1558,20 +1483,20 @@
         <v>86</v>
       </c>
       <c r="G2">
-        <v>85.207300000000004</v>
+        <v>85.272300000000001</v>
       </c>
       <c r="H2">
-        <v>86.247</v>
+        <v>86.396000000000001</v>
       </c>
       <c r="I2">
-        <v>1285</v>
+        <v>685</v>
       </c>
       <c r="J2">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="K2">
         <f>(H2-G2)/H2</f>
-        <v>1.2054912054912012E-2</v>
+        <v>1.3006389184684469E-2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1591,62 +1516,62 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
@@ -1656,567 +1581,452 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>127</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>166</v>
+        <v>100</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>168</v>
+        <v>101</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>171</v>
+        <v>102</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>172</v>
+        <v>103</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
-        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>